<commit_message>
Working on 2023 report
</commit_message>
<xml_diff>
--- a/Data/wtryrtype.xlsx
+++ b/Data/wtryrtype.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/rosemary_hartman_water_ca_gov/Documents/salinity control gates/SMSCG/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/rosemary_hartman_water_ca_gov/Documents/salinity control gates/SMSCG/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E82DFE74-879D-4857-B0A2-7C16A8805E3D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{E82DFE74-879D-4857-B0A2-7C16A8805E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFCB478B-59A4-43CE-862E-B2D207CF5A99}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18915" windowHeight="6000" xr2:uid="{FFC84A21-9A32-4503-836D-92B86F6012D5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{FFC84A21-9A32-4503-836D-92B86F6012D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="11">
   <si>
     <t>WY</t>
   </si>
@@ -418,15 +418,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{285FF48E-1B64-4A88-8BF9-D3613EE5AE38}">
-  <dimension ref="A1:F114"/>
+  <dimension ref="A1:F119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="F120" sqref="F120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -446,7 +446,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1906</v>
       </c>
@@ -466,7 +466,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1907</v>
       </c>
@@ -486,7 +486,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1908</v>
       </c>
@@ -506,7 +506,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1909</v>
       </c>
@@ -526,7 +526,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>1910</v>
       </c>
@@ -546,7 +546,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>1911</v>
       </c>
@@ -566,7 +566,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>1912</v>
       </c>
@@ -586,7 +586,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>1913</v>
       </c>
@@ -606,7 +606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>1914</v>
       </c>
@@ -626,7 +626,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>1915</v>
       </c>
@@ -646,7 +646,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>1916</v>
       </c>
@@ -666,7 +666,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>1917</v>
       </c>
@@ -686,7 +686,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>1918</v>
       </c>
@@ -706,7 +706,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>1919</v>
       </c>
@@ -726,7 +726,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>1920</v>
       </c>
@@ -746,7 +746,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>1921</v>
       </c>
@@ -766,7 +766,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>1922</v>
       </c>
@@ -786,7 +786,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>1923</v>
       </c>
@@ -806,7 +806,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>1924</v>
       </c>
@@ -826,7 +826,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>1925</v>
       </c>
@@ -846,7 +846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>1926</v>
       </c>
@@ -866,7 +866,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>1927</v>
       </c>
@@ -886,7 +886,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>1928</v>
       </c>
@@ -906,7 +906,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>1929</v>
       </c>
@@ -926,7 +926,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>1930</v>
       </c>
@@ -946,7 +946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>1931</v>
       </c>
@@ -966,7 +966,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>1932</v>
       </c>
@@ -986,7 +986,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>1933</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>1934</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>1935</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>1936</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>1937</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>1938</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>1939</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>1940</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>1941</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>1942</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>1943</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>1944</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>1945</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>1946</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>1947</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>1948</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>1949</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>1950</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>1951</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>1952</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>1953</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>1954</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>1955</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>1956</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>1957</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>1958</v>
       </c>
@@ -1506,7 +1506,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>1959</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>1960</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>1961</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>1962</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>1963</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>1964</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>1965</v>
       </c>
@@ -1646,7 +1646,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>1966</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>1967</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>1968</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>1969</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>1970</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>1971</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>1972</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>1973</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>1974</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>1975</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>1976</v>
       </c>
@@ -1866,7 +1866,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>1977</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>1978</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>1979</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>1980</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>1981</v>
       </c>
@@ -1966,7 +1966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>1982</v>
       </c>
@@ -1986,7 +1986,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>1983</v>
       </c>
@@ -2006,7 +2006,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>1984</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>1985</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>1986</v>
       </c>
@@ -2066,7 +2066,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>1987</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>1988</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>1989</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>1990</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>1991</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>1992</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>1993</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>1994</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>1995</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>1996</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <v>1997</v>
       </c>
@@ -2286,7 +2286,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <v>1998</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>1999</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>2000</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <v>2001</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>2002</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>2003</v>
       </c>
@@ -2406,7 +2406,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>2004</v>
       </c>
@@ -2426,7 +2426,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>2005</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>2006</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>2007</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
         <v>2008</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
         <v>2009</v>
       </c>
@@ -2526,7 +2526,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
         <v>2010</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
         <v>2011</v>
       </c>
@@ -2566,7 +2566,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
         <v>2012</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
         <v>2013</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
         <v>2014</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
         <v>2015</v>
       </c>
@@ -2646,7 +2646,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
         <v>2016</v>
       </c>
@@ -2666,7 +2666,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
         <v>2017</v>
       </c>
@@ -2686,7 +2686,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
         <v>2018</v>
       </c>
@@ -2704,6 +2704,61 @@
       </c>
       <c r="F114" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A115" s="1">
+        <v>2019</v>
+      </c>
+      <c r="E115">
+        <v>10.34</v>
+      </c>
+      <c r="F115" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A116" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E116">
+        <v>6.13</v>
+      </c>
+      <c r="F116" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A117" s="1">
+        <v>2021</v>
+      </c>
+      <c r="E117">
+        <v>3.86</v>
+      </c>
+      <c r="F117" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A118" s="1">
+        <v>2022</v>
+      </c>
+      <c r="E118">
+        <v>4.5</v>
+      </c>
+      <c r="F118" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A119" s="1">
+        <v>2023</v>
+      </c>
+      <c r="E119">
+        <v>9.35</v>
+      </c>
+      <c r="F119" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>